<commit_message>
Desarrollado un script que envia un correo a una dirección con 1 adjunto
ToDo: Hacer que el script envíe varios adjunto y que lo haga a múltiples destinatarios
</commit_message>
<xml_diff>
--- a/SHAMPOO COLAGENO.xlsx
+++ b/SHAMPOO COLAGENO.xlsx
@@ -393,6 +393,9 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
@@ -422,9 +425,6 @@
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
@@ -478,7 +478,7 @@
     <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
     <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -488,16 +488,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -799,10 +789,10 @@
   </sheetPr>
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="M1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="K1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" xSplit="0" ySplit="1"/>
-      <selection activeCell="M1" activeCellId="0" pane="topLeft" sqref="M1"/>
-      <selection activeCell="R3" activeCellId="0" pane="bottomLeft" sqref="R3:R36"/>
+      <selection activeCell="K1" activeCellId="0" pane="topLeft" sqref="K1"/>
+      <selection activeCell="R6" activeCellId="0" pane="bottomLeft" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
@@ -934,7 +924,7 @@
       <c r="Q2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="27" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1330,7 +1320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="10" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="10" s="19" spans="1:18">
       <c r="A10" s="14" t="n">
         <v>43211</v>
       </c>
@@ -1386,7 +1376,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="11" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="11" s="19" spans="1:18">
       <c r="A11" s="14" t="n">
         <v>43211</v>
       </c>
@@ -1442,7 +1432,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="12" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="12" s="19" spans="1:18">
       <c r="A12" s="14" t="n">
         <v>43211</v>
       </c>
@@ -1498,7 +1488,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="13" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="13" s="19" spans="1:18">
       <c r="A13" s="14" t="n">
         <v>43211</v>
       </c>
@@ -1554,7 +1544,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="14" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="14" s="19" spans="1:18">
       <c r="A14" s="14" t="n">
         <v>43211</v>
       </c>
@@ -1610,7 +1600,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="15" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="15" s="19" spans="1:18">
       <c r="A15" s="14" t="n">
         <v>43211</v>
       </c>
@@ -1666,7 +1656,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="16" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="16" s="19" spans="1:18">
       <c r="A16" s="14" t="n">
         <v>43222</v>
       </c>
@@ -1722,7 +1712,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="17" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="17" s="19" spans="1:18">
       <c r="A17" s="14" t="n">
         <v>43222</v>
       </c>
@@ -1778,7 +1768,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="18" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="18" s="19" spans="1:18">
       <c r="A18" s="14" t="n">
         <v>43236</v>
       </c>
@@ -1834,7 +1824,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="19" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="19" s="19" spans="1:18">
       <c r="A19" s="14" t="n">
         <v>43236</v>
       </c>
@@ -1890,7 +1880,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="20" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="20" s="19" spans="1:18">
       <c r="A20" s="14" t="n">
         <v>43236</v>
       </c>
@@ -1946,7 +1936,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="21" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="21" s="19" spans="1:18">
       <c r="A21" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2002,7 +1992,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="22" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="22" s="19" spans="1:18">
       <c r="A22" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2058,7 +2048,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="23" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="23" s="19" spans="1:18">
       <c r="A23" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2114,7 +2104,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="24" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="24" s="19" spans="1:18">
       <c r="A24" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2170,7 +2160,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="25" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="25" s="19" spans="1:18">
       <c r="A25" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2226,7 +2216,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="26" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="26" s="19" spans="1:18">
       <c r="A26" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2282,7 +2272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="27" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="27" s="19" spans="1:18">
       <c r="A27" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2338,7 +2328,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="28" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="28" s="19" spans="1:18">
       <c r="A28" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2394,7 +2384,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="29" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="29" s="19" spans="1:18">
       <c r="A29" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2450,7 +2440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="30" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="30" s="19" spans="1:18">
       <c r="A30" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2506,7 +2496,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="31" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="31" s="19" spans="1:18">
       <c r="A31" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2562,7 +2552,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="32" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="32" s="19" spans="1:18">
       <c r="A32" s="14" t="n">
         <v>43236</v>
       </c>
@@ -2618,7 +2608,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="33" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="33" s="19" spans="1:18">
       <c r="A33" s="14" t="n">
         <v>43242</v>
       </c>
@@ -2674,7 +2664,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="34" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="34" s="19" spans="1:18">
       <c r="A34" s="14" t="n">
         <v>43242</v>
       </c>
@@ -2730,7 +2720,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="35" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="35" s="19" spans="1:18">
       <c r="A35" s="14" t="n">
         <v>43242</v>
       </c>
@@ -2786,7 +2776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="36" s="19" spans="1:18">
+    <row customHeight="1" ht="14.9" r="36" s="19" spans="1:18">
       <c r="A36" s="14" t="n">
         <v>43242</v>
       </c>
@@ -3401,7 +3391,7 @@
   <dimension ref="B3:C4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B4" activeCellId="1" pane="topLeft" sqref="R3:R36 B4"/>
+      <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>

</xml_diff>